<commit_message>
Added taskes in excel
</commit_message>
<xml_diff>
--- a/tiempo de tareas.xlsx
+++ b/tiempo de tareas.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferranrogerbib\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9630"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Tasca</t>
   </si>
@@ -39,13 +34,37 @@
   </si>
   <si>
     <t>5 h</t>
+  </si>
+  <si>
+    <t>Persona Encarregada</t>
+  </si>
+  <si>
+    <t>Fer Welcome Page</t>
+  </si>
+  <si>
+    <t>Canviar spritesheets escenaris Handout</t>
+  </si>
+  <si>
+    <t>Fer End Battle Screen</t>
+  </si>
+  <si>
+    <t>Maquetar proyecte final per fer les tasques Handout 5</t>
+  </si>
+  <si>
+    <t>Rafa</t>
+  </si>
+  <si>
+    <t>1:30 h</t>
+  </si>
+  <si>
+    <t>1 h</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,16 +72,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -70,17 +102,299 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Celda de comprobación" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="9">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="double">
+          <color rgb="FF3F3F3F"/>
+        </left>
+        <right/>
+        <top style="double">
+          <color rgb="FF3F3F3F"/>
+        </top>
+        <bottom style="double">
+          <color rgb="FF3F3F3F"/>
+        </bottom>
+        <vertical style="double">
+          <color rgb="FF3F3F3F"/>
+        </vertical>
+        <horizontal style="double">
+          <color rgb="FF3F3F3F"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="double">
+          <color rgb="FF3F3F3F"/>
+        </left>
+        <right style="double">
+          <color rgb="FF3F3F3F"/>
+        </right>
+        <top style="double">
+          <color rgb="FF3F3F3F"/>
+        </top>
+        <bottom style="double">
+          <color rgb="FF3F3F3F"/>
+        </bottom>
+        <vertical style="double">
+          <color rgb="FF3F3F3F"/>
+        </vertical>
+        <horizontal style="double">
+          <color rgb="FF3F3F3F"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="double">
+          <color rgb="FF3F3F3F"/>
+        </left>
+        <right style="double">
+          <color rgb="FF3F3F3F"/>
+        </right>
+        <top style="double">
+          <color rgb="FF3F3F3F"/>
+        </top>
+        <bottom style="double">
+          <color rgb="FF3F3F3F"/>
+        </bottom>
+        <vertical style="double">
+          <color rgb="FF3F3F3F"/>
+        </vertical>
+        <horizontal style="double">
+          <color rgb="FF3F3F3F"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="double">
+          <color rgb="FF3F3F3F"/>
+        </right>
+        <top style="double">
+          <color rgb="FF3F3F3F"/>
+        </top>
+        <bottom style="double">
+          <color rgb="FF3F3F3F"/>
+        </bottom>
+        <vertical style="double">
+          <color rgb="FF3F3F3F"/>
+        </vertical>
+        <horizontal style="double">
+          <color rgb="FF3F3F3F"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="double">
+          <color rgb="FF3F3F3F"/>
+        </left>
+        <right style="double">
+          <color rgb="FF3F3F3F"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="double">
+          <color rgb="FF3F3F3F"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="double">
+          <color rgb="FF3F3F3F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="double">
+          <color rgb="FF3F3F3F"/>
+        </left>
+        <right style="double">
+          <color rgb="FF3F3F3F"/>
+        </right>
+        <top style="double">
+          <color rgb="FF3F3F3F"/>
+        </top>
+        <bottom style="double">
+          <color rgb="FF3F3F3F"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -91,6 +405,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A2:D40" totalsRowShown="0" headerRowDxfId="5" dataDxfId="0" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6" headerRowCellStyle="Celda de comprobación">
+  <autoFilter ref="A2:D40"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Tasca" dataDxfId="4"/>
+    <tableColumn id="2" name="Persona Encarregada" dataDxfId="3"/>
+    <tableColumn id="3" name="Previsió" dataDxfId="2"/>
+    <tableColumn id="4" name="Temps" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -136,7 +463,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -171,7 +498,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -348,46 +675,291 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+    <col min="1" max="1" width="36.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="3" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6" t="s">
         <v>4</v>
       </c>
+    </row>
+    <row r="4" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="1:4" ht="31.5" thickTop="1" thickBot="1">
+      <c r="A15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="6"/>
+    </row>
+    <row r="20" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="6"/>
+    </row>
+    <row r="21" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="6"/>
+    </row>
+    <row r="22" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="6"/>
+    </row>
+    <row r="23" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="6"/>
+    </row>
+    <row r="24" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="6"/>
+    </row>
+    <row r="25" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A25" s="4"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="6"/>
+    </row>
+    <row r="26" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A26" s="4"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="6"/>
+    </row>
+    <row r="27" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A27" s="4"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="6"/>
+    </row>
+    <row r="28" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A28" s="4"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="6"/>
+    </row>
+    <row r="29" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A29" s="4"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="6"/>
+    </row>
+    <row r="30" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A30" s="4"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="6"/>
+    </row>
+    <row r="31" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A31" s="4"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="6"/>
+    </row>
+    <row r="32" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A32" s="4"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="6"/>
+    </row>
+    <row r="33" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A33" s="4"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="6"/>
+    </row>
+    <row r="34" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A34" s="4"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="6"/>
+    </row>
+    <row r="35" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A35" s="4"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="6"/>
+    </row>
+    <row r="36" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A36" s="4"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="6"/>
+    </row>
+    <row r="37" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A37" s="4"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="6"/>
+    </row>
+    <row r="38" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A38" s="4"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="6"/>
+    </row>
+    <row r="39" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A39" s="4"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="6"/>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" thickTop="1">
+      <c r="A40" s="7"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Maquetar Handout 5 y hacer welcome y post fight pages
</commit_message>
<xml_diff>
--- a/tiempo de tareas.xlsx
+++ b/tiempo de tareas.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Tasca</t>
   </si>
@@ -57,7 +57,16 @@
     <t>1:30 h</t>
   </si>
   <si>
-    <t>1 h</t>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>0:30 h</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>0:20 h</t>
   </si>
 </sst>
 </file>
@@ -258,9 +267,6 @@
   <dxfs count="9">
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="double">
           <color rgb="FF3F3F3F"/>
@@ -348,32 +354,10 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="double">
-          <color rgb="FF3F3F3F"/>
-        </left>
-        <right style="double">
-          <color rgb="FF3F3F3F"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <border>
         <top style="double">
           <color rgb="FF3F3F3F"/>
         </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="double">
-          <color rgb="FF3F3F3F"/>
-        </bottom>
         <vertical/>
         <horizontal/>
       </border>
@@ -392,6 +376,31 @@
         <bottom style="double">
           <color rgb="FF3F3F3F"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="double">
+          <color rgb="FF3F3F3F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="double">
+          <color rgb="FF3F3F3F"/>
+        </left>
+        <right style="double">
+          <color rgb="FF3F3F3F"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -408,13 +417,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A2:D40" totalsRowShown="0" headerRowDxfId="5" dataDxfId="0" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6" headerRowCellStyle="Celda de comprobación">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A2:D40" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4" headerRowCellStyle="Celda de comprobación">
   <autoFilter ref="A2:D40"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Tasca" dataDxfId="4"/>
-    <tableColumn id="2" name="Persona Encarregada" dataDxfId="3"/>
-    <tableColumn id="3" name="Previsió" dataDxfId="2"/>
-    <tableColumn id="4" name="Temps" dataDxfId="1"/>
+    <tableColumn id="1" name="Tasca" dataDxfId="3"/>
+    <tableColumn id="2" name="Persona Encarregada" dataDxfId="2"/>
+    <tableColumn id="3" name="Previsió" dataDxfId="1"/>
+    <tableColumn id="4" name="Temps" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -675,7 +684,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -686,7 +695,7 @@
   <dimension ref="A2:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -803,9 +812,15 @@
       <c r="A16" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
+      <c r="B16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="17" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
       <c r="A17" s="4" t="s">
@@ -819,9 +834,15 @@
       <c r="A18" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
+      <c r="B18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="19" spans="1:4" ht="16.5" thickTop="1" thickBot="1">
       <c r="A19" s="4"/>

</xml_diff>

<commit_message>
Añadido Hadoken y su respectivo sonido.
</commit_message>
<xml_diff>
--- a/tiempo de tareas.xlsx
+++ b/tiempo de tareas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t xml:space="preserve">Tasca</t>
   </si>
@@ -64,6 +64,21 @@
     <t xml:space="preserve">0:30 h</t>
   </si>
   <si>
+    <t xml:space="preserve">Hacer Hadoken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modulo player 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jose, Ferran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1h</t>
+  </si>
+  <si>
     <t xml:space="preserve">Maquetar proyecte final per fer les tasques Handout 5</t>
   </si>
   <si>
@@ -73,13 +88,7 @@
     <t xml:space="preserve">1:30 h</t>
   </si>
   <si>
-    <t xml:space="preserve">2h</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fer Welcome Page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1h</t>
   </si>
   <si>
     <t xml:space="preserve">Canviar spritesheets escenaris Handout</t>
@@ -449,12 +458,12 @@
   <dimension ref="A2:D40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="23.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="10.71"/>
   </cols>
@@ -512,16 +521,32 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
+      <c r="A6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4"/>
@@ -567,35 +592,35 @@
     </row>
     <row r="15" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -603,30 +628,30 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -637,7 +662,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>11</v>
@@ -649,30 +674,30 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="6"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="6"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="6"/>

</xml_diff>

<commit_message>
Añadir horas de tareas
</commit_message>
<xml_diff>
--- a/tiempo de tareas.xlsx
+++ b/tiempo de tareas.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,113 +19,118 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
-  <si>
-    <t xml:space="preserve">Tasca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Persona Encarregada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Previsió</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fer mòdul background per l'scroll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Añadir musica modulos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ferran, Jose, Adriá</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arreglar Salto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0:30 h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hacer Hadoken</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modulo player 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jose, Ferran</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maquetar proyecte final per fer les tasques Handout 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rafa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1:30 h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fer Welcome Page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Canviar spritesheets escenaris Handout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fer End Battle Screen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0:20 h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Corregir errores del commit Ferrán</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0:45 h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cosas varias</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adriá</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ferran</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
+  <si>
+    <t>Tasca</t>
+  </si>
+  <si>
+    <t>Persona Encarregada</t>
+  </si>
+  <si>
+    <t>Previsió</t>
+  </si>
+  <si>
+    <t>Temps</t>
+  </si>
+  <si>
+    <t>Fer mòdul background per l'scroll</t>
+  </si>
+  <si>
+    <t>5 h</t>
+  </si>
+  <si>
+    <t>Añadir musica modulos</t>
+  </si>
+  <si>
+    <t>Ferran, Jose, Adriá</t>
+  </si>
+  <si>
+    <t>2 h</t>
+  </si>
+  <si>
+    <t>3 h</t>
+  </si>
+  <si>
+    <t>Arreglar Salto</t>
+  </si>
+  <si>
+    <t>Jose</t>
+  </si>
+  <si>
+    <t>1 h</t>
+  </si>
+  <si>
+    <t>0:30 h</t>
+  </si>
+  <si>
+    <t>Hacer Hadoken</t>
+  </si>
+  <si>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>Modulo player 2</t>
+  </si>
+  <si>
+    <t>Jose, Ferran</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>Maquetar proyecte final per fer les tasques Handout 5</t>
+  </si>
+  <si>
+    <t>Rafa</t>
+  </si>
+  <si>
+    <t>1:30 h</t>
+  </si>
+  <si>
+    <t>Fer Welcome Page</t>
+  </si>
+  <si>
+    <t>Canviar spritesheets escenaris Handout</t>
+  </si>
+  <si>
+    <t>Fer End Battle Screen</t>
+  </si>
+  <si>
+    <t>0:20 h</t>
+  </si>
+  <si>
+    <t>Corregir errores del commit Ferrán</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>0:45 h</t>
+  </si>
+  <si>
+    <t>Cosas varias</t>
+  </si>
+  <si>
+    <t>Adriá</t>
+  </si>
+  <si>
+    <t>Ferran</t>
+  </si>
+  <si>
+    <t>Añadir Fade out fade in</t>
+  </si>
+  <si>
+    <t>Añadir modulos handout 7</t>
+  </si>
+  <si>
+    <t>Añadir objeto frame</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="H:MM"/>
-  </numFmts>
-  <fonts count="5">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -135,22 +139,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -173,14 +162,14 @@
     </fill>
   </fills>
   <borders count="10">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -195,7 +184,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right style="double">
         <color rgb="FF3F3F3F"/>
@@ -206,7 +195,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -219,7 +208,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -230,7 +219,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right style="double">
         <color rgb="FF3F3F3F"/>
@@ -243,7 +232,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -256,7 +245,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right style="double">
         <color rgb="FF3F3F3F"/>
@@ -267,7 +256,7 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -280,7 +269,7 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -292,89 +281,55 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="2">
+    <cellStyle name="Excel Built-in Check Cell" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Excel Built-in Check Cell" xfId="20"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -433,13 +388,21 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A2:D40" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A2:D40" totalsRowShown="0">
   <autoFilter ref="A2:D40"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Tasca"/>
@@ -447,28 +410,309 @@
     <tableColumn id="3" name="Previsió"/>
     <tableColumn id="4" name="Temps"/>
   </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A2:D40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="23.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="10.71"/>
+    <col min="1" max="1" width="36.28515625" customWidth="1"/>
+    <col min="2" max="3" width="23" customWidth="1"/>
+    <col min="4" max="1025" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -482,7 +726,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:4">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -492,7 +736,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:4">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -506,7 +750,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:4">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
@@ -520,7 +764,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:4">
       <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
@@ -534,7 +778,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:4">
       <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
@@ -548,49 +792,57 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:4">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:4">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:4">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:4">
+      <c r="A11" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:4">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:4">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:4" ht="30">
       <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
@@ -604,7 +856,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:4">
       <c r="A16" s="4" t="s">
         <v>22</v>
       </c>
@@ -618,7 +870,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:4">
       <c r="A17" s="4" t="s">
         <v>23</v>
       </c>
@@ -626,7 +878,7 @@
       <c r="C17" s="5"/>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:4">
       <c r="A18" s="4" t="s">
         <v>24</v>
       </c>
@@ -640,7 +892,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:4">
       <c r="A19" s="4" t="s">
         <v>26</v>
       </c>
@@ -654,13 +906,21 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:4">
+      <c r="A20" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="4" t="s">
         <v>29</v>
       </c>
@@ -672,7 +932,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:4">
       <c r="A22" s="4" t="s">
         <v>29</v>
       </c>
@@ -682,7 +942,7 @@
       <c r="C22" s="5"/>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:4">
       <c r="A23" s="4" t="s">
         <v>29</v>
       </c>
@@ -692,7 +952,7 @@
       <c r="C23" s="5"/>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:4">
       <c r="A24" s="4" t="s">
         <v>29</v>
       </c>
@@ -702,111 +962,114 @@
       <c r="C24" s="5"/>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="6"/>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:4">
+      <c r="A25" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="6"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:4">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="6"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:4">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:4">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:4">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:4">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="6"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:4">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="6"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:4">
       <c r="A33" s="4"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:4">
       <c r="A34" s="4"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="6"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:4">
       <c r="A35" s="4"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="6"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:4">
       <c r="A36" s="4"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="6"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:4">
       <c r="A37" s="4"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="6"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:4">
       <c r="A38" s="4"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="6"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:4">
       <c r="A39" s="4"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="6"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:4">
       <c r="A40" s="8"/>
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
       <c r="D40" s="10"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <tableParts>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>

</xml_diff>

<commit_message>
I ate a merge, camera fixation completed
</commit_message>
<xml_diff>
--- a/tiempo de tareas.xlsx
+++ b/tiempo de tareas.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ferba93\Documents\GitHub\Street-Fighter-II-Gamusinos-Fighters-\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,131 +24,142 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
-  <si>
-    <t xml:space="preserve">Tasca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Persona Encarregada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Previsió</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fer mòdul background per l'scroll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Añadir musica modulos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ferran, Jose, Adriá</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arreglar Salto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0:30 h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hacer Hadoken</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modulo player 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jose, Ferran</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hitbox hdk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0:30h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0:45 h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Golpear al oponente con hdk y animacion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Añadir Fade out fade in</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adriá</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maquetar proyecte final per fer les tasques Handout 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rafa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1:30 h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fer Welcome Page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Canviar spritesheets escenaris Handout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fer End Battle Screen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0:20 h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Corregir errores del commit Ferrán</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Añadir modulos handout 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cosas varias</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ferran</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Añadir objeto frame</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="43">
+  <si>
+    <t>Tasca</t>
+  </si>
+  <si>
+    <t>Persona Encarregada</t>
+  </si>
+  <si>
+    <t>Previsió</t>
+  </si>
+  <si>
+    <t>Temps</t>
+  </si>
+  <si>
+    <t>Fer mòdul background per l'scroll</t>
+  </si>
+  <si>
+    <t>5 h</t>
+  </si>
+  <si>
+    <t>Añadir musica modulos</t>
+  </si>
+  <si>
+    <t>Ferran, Jose, Adriá</t>
+  </si>
+  <si>
+    <t>2 h</t>
+  </si>
+  <si>
+    <t>3 h</t>
+  </si>
+  <si>
+    <t>Arreglar Salto</t>
+  </si>
+  <si>
+    <t>Jose</t>
+  </si>
+  <si>
+    <t>1 h</t>
+  </si>
+  <si>
+    <t>0:30 h</t>
+  </si>
+  <si>
+    <t>Hacer Hadoken</t>
+  </si>
+  <si>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>Modulo player 2</t>
+  </si>
+  <si>
+    <t>Jose, Ferran</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>Hitbox hdk</t>
+  </si>
+  <si>
+    <t>0:30h</t>
+  </si>
+  <si>
+    <t>0:45 h</t>
+  </si>
+  <si>
+    <t>Golpear al oponente con hdk y animacion</t>
+  </si>
+  <si>
+    <t>Añadir Fade out fade in</t>
+  </si>
+  <si>
+    <t>Adriá</t>
+  </si>
+  <si>
+    <t>Maquetar proyecte final per fer les tasques Handout 5</t>
+  </si>
+  <si>
+    <t>Rafa</t>
+  </si>
+  <si>
+    <t>1:30 h</t>
+  </si>
+  <si>
+    <t>Fer Welcome Page</t>
+  </si>
+  <si>
+    <t>Canviar spritesheets escenaris Handout</t>
+  </si>
+  <si>
+    <t>Fer End Battle Screen</t>
+  </si>
+  <si>
+    <t>0:20 h</t>
+  </si>
+  <si>
+    <t>Corregir errores del commit Ferrán</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Añadir modulos handout 7</t>
+  </si>
+  <si>
+    <t>Cosas varias</t>
+  </si>
+  <si>
+    <t>Ferran</t>
+  </si>
+  <si>
+    <t>Añadir objeto frame</t>
+  </si>
+  <si>
+    <t>10 min</t>
+  </si>
+  <si>
+    <t>15 min</t>
+  </si>
+  <si>
+    <t>Fijar la cámara</t>
+  </si>
+  <si>
+    <t>4 h</t>
+  </si>
+  <si>
+    <t>Hacer colisiones con proyectiles</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="H:MM"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -153,24 +168,17 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -191,14 +199,14 @@
     </fill>
   </fills>
   <borders count="10">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -213,7 +221,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right style="double">
         <color rgb="FF3F3F3F"/>
@@ -224,7 +232,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -237,7 +245,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -248,7 +256,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right style="double">
         <color rgb="FF3F3F3F"/>
@@ -261,7 +269,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -274,7 +282,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right style="double">
         <color rgb="FF3F3F3F"/>
@@ -285,7 +293,7 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -298,7 +306,7 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -310,89 +318,52 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="2">
+    <cellStyle name="Excel Built-in Check Cell" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Excel Built-in Check Cell" xfId="20"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -451,13 +422,29 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A2:D40" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A2:D40" totalsRowShown="0">
   <autoFilter ref="A2:D40"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Tasca"/>
@@ -465,28 +452,287 @@
     <tableColumn id="3" name="Previsió"/>
     <tableColumn id="4" name="Temps"/>
   </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N8" activeCellId="0" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="23.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="10.71"/>
+    <col min="1" max="1" width="36.28515625" customWidth="1"/>
+    <col min="2" max="3" width="23" customWidth="1"/>
+    <col min="4" max="1025" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -500,7 +746,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -510,7 +756,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -524,7 +770,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
@@ -538,7 +784,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
@@ -552,7 +798,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
@@ -566,7 +812,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>19</v>
       </c>
@@ -580,7 +826,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>22</v>
       </c>
@@ -592,13 +838,13 @@
       </c>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
@@ -612,25 +858,25 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>25</v>
       </c>
@@ -644,7 +890,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>28</v>
       </c>
@@ -658,7 +904,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>29</v>
       </c>
@@ -666,7 +912,7 @@
       <c r="C17" s="5"/>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>30</v>
       </c>
@@ -680,7 +926,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>32</v>
       </c>
@@ -694,7 +940,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>34</v>
       </c>
@@ -708,7 +954,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>35</v>
       </c>
@@ -720,7 +966,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>35</v>
       </c>
@@ -730,17 +976,21 @@
       <c r="C22" s="5"/>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="6"/>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>35</v>
       </c>
@@ -750,7 +1000,7 @@
       <c r="C24" s="5"/>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>37</v>
       </c>
@@ -764,106 +1014,117 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="6"/>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="6"/>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="6"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="6"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="6"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="6"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="6"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="6"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="6"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="6"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
       <c r="D40" s="10"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <tableParts>
-    <tablePart r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>